<commit_message>
Removes unused core class
Removes a default core class that is no longer needed, cleaning up the project structure.

Updates error codes.
</commit_message>
<xml_diff>
--- a/ErrorCodes.xlsx
+++ b/ErrorCodes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zamos\Documents\GitHub\CtrlPay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE317EBA-6746-475A-AF40-AAE1DFB7EABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD3C4286-FFFE-46DF-8DE7-62AA3A0405F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>ErrorCode</t>
   </si>
@@ -46,6 +46,15 @@
   </si>
   <si>
     <t>wrong password</t>
+  </si>
+  <si>
+    <t>user does not exists</t>
+  </si>
+  <si>
+    <t>totp not valid</t>
+  </si>
+  <si>
+    <t>login valid, awaiting totp auth</t>
   </si>
 </sst>
 </file>
@@ -363,10 +372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B8:B9"/>
+      <selection activeCell="E18" sqref="D18:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -413,6 +422,30 @@
         <v>6</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: Enhance ReturnModel with DetailMessage and new error codes
</commit_message>
<xml_diff>
--- a/ErrorCodes.xlsx
+++ b/ErrorCodes.xlsx
@@ -1,50 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coufalkrystof\Desktop\CtrlPay\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zamos\Documents\GitHub\CtrlPay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{111F7938-F7EB-44C6-BAD5-0B365D34C226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DECB938-6466-4E94-86D3-D5605EC1C4F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37965" yWindow="5955" windowWidth="28800" windowHeight="15345" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="List1" sheetId="1" r:id="rId1"/>
-    <sheet name="List2" sheetId="2" r:id="rId2"/>
+    <sheet name="Auth" sheetId="2" r:id="rId1"/>
+    <sheet name="Payments" sheetId="6" r:id="rId2"/>
+    <sheet name="Register" sheetId="3" r:id="rId3"/>
+    <sheet name="Transactions" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
-      <xlwcv:version setVersion="1"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
-  <si>
-    <t>ErrorCode</t>
-  </si>
-  <si>
-    <t>StandardMessage</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>success</t>
-  </si>
-  <si>
-    <t>vše proběhlo bez chyby</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="87">
   <si>
     <t>user with the same username already exists</t>
   </si>
@@ -52,9 +36,6 @@
     <t>wrong password</t>
   </si>
   <si>
-    <t>user does not exists</t>
-  </si>
-  <si>
     <t>totp not valid</t>
   </si>
   <si>
@@ -134,6 +115,180 @@
   </si>
   <si>
     <t>token is not totp token</t>
+  </si>
+  <si>
+    <t>HTTP error code received</t>
+  </si>
+  <si>
+    <t>Severity</t>
+  </si>
+  <si>
+    <t>Register Error Codes</t>
+  </si>
+  <si>
+    <t>R#</t>
+  </si>
+  <si>
+    <t>R0</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>R9</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>R15</t>
+  </si>
+  <si>
+    <t>successfully registered</t>
+  </si>
+  <si>
+    <t>T0</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>T3</t>
+  </si>
+  <si>
+    <t>T4</t>
+  </si>
+  <si>
+    <t>T5</t>
+  </si>
+  <si>
+    <t>T6</t>
+  </si>
+  <si>
+    <t>T7</t>
+  </si>
+  <si>
+    <t>T8</t>
+  </si>
+  <si>
+    <t>T9</t>
+  </si>
+  <si>
+    <t>T10</t>
+  </si>
+  <si>
+    <t>T11</t>
+  </si>
+  <si>
+    <t>T12</t>
+  </si>
+  <si>
+    <t>T13</t>
+  </si>
+  <si>
+    <t>T14</t>
+  </si>
+  <si>
+    <t>T15</t>
+  </si>
+  <si>
+    <t>operation succesful</t>
+  </si>
+  <si>
+    <t>T#</t>
+  </si>
+  <si>
+    <t>Transactions Error Codes</t>
+  </si>
+  <si>
+    <t>Payments Error Codes</t>
+  </si>
+  <si>
+    <t>P#</t>
+  </si>
+  <si>
+    <t>P0</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>P4</t>
+  </si>
+  <si>
+    <t>P5</t>
+  </si>
+  <si>
+    <t>P6</t>
+  </si>
+  <si>
+    <t>P7</t>
+  </si>
+  <si>
+    <t>P8</t>
+  </si>
+  <si>
+    <t>P9</t>
+  </si>
+  <si>
+    <t>P10</t>
+  </si>
+  <si>
+    <t>P11</t>
+  </si>
+  <si>
+    <t>P12</t>
+  </si>
+  <si>
+    <t>P13</t>
+  </si>
+  <si>
+    <t>P14</t>
+  </si>
+  <si>
+    <t>P15</t>
   </si>
 </sst>
 </file>
@@ -181,7 +336,112 @@
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="18">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -478,92 +738,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
-  <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="B7" sqref="B3:B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9E7729A-1ECD-4D18-AD79-215030F792F8}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,157 +754,587 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
         <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="containsText" dxfId="17" priority="1" operator="containsText" text="OK">
+      <formula>NOT(ISERROR(SEARCH("OK",C1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="2" operator="containsText" text="WARNING">
+      <formula>NOT(ISERROR(SEARCH("WARNING",C1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="15" priority="3" operator="containsText" text="ERROR">
+      <formula>NOT(ISERROR(SEARCH("ERROR",C1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB5244BA-F464-4FCB-913B-51EE1447A6F5}">
+  <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="C1:C2 C4:C1048576">
+    <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="OK">
+      <formula>NOT(ISERROR(SEARCH("OK",C1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="5" operator="containsText" text="WARNING">
+      <formula>NOT(ISERROR(SEARCH("WARNING",C1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="ERROR">
+      <formula>NOT(ISERROR(SEARCH("ERROR",C1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="OK">
+      <formula>NOT(ISERROR(SEARCH("OK",C3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="WARNING">
+      <formula>NOT(ISERROR(SEARCH("WARNING",C3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="ERROR">
+      <formula>NOT(ISERROR(SEARCH("ERROR",C3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49F1D35A-F5B1-4F7C-BEBF-5839D23DDC9A}">
+  <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B7" sqref="A1:C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="containsText" dxfId="14" priority="1" operator="containsText" text="OK">
+      <formula>NOT(ISERROR(SEARCH("OK",C1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="2" operator="containsText" text="WARNING">
+      <formula>NOT(ISERROR(SEARCH("WARNING",C1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="3" operator="containsText" text="ERROR">
+      <formula>NOT(ISERROR(SEARCH("ERROR",C1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7718E203-9D51-4778-8682-1A55B2CB558B}">
+  <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="C1:C2 C4:C1048576">
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="OK">
+      <formula>NOT(ISERROR(SEARCH("OK",C1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="WARNING">
+      <formula>NOT(ISERROR(SEARCH("WARNING",C1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="ERROR">
+      <formula>NOT(ISERROR(SEARCH("ERROR",C1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="OK">
+      <formula>NOT(ISERROR(SEARCH("OK",C3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="WARNING">
+      <formula>NOT(ISERROR(SEARCH("WARNING",C3)))</formula>
+    </cfRule>
     <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="ERROR">
-      <formula>NOT(ISERROR(SEARCH("ERROR",C1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="WARNING">
-      <formula>NOT(ISERROR(SEARCH("WARNING",C1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="OK">
-      <formula>NOT(ISERROR(SEARCH("OK",C1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("ERROR",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adds transaction view to navbar
Adds a transaction view with sorting options to the navbar.
Implements RangeObservableCollection for efficient list updates in UI.
Moves SortOption and RangeObservableCollection classes to HelperClasses.
Adds cash icon.
</commit_message>
<xml_diff>
--- a/ErrorCodes.xlsx
+++ b/ErrorCodes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zamos\Documents\GitHub\CtrlPay\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CtrlPay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DECB938-6466-4E94-86D3-D5605EC1C4F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{283E9023-256D-44BF-BFCD-43F5BD86C280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37965" yWindow="5955" windowWidth="28800" windowHeight="15345" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="2970" windowWidth="29040" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Auth" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="89">
   <si>
     <t>user with the same username already exists</t>
   </si>
@@ -289,6 +289,12 @@
   </si>
   <si>
     <t>P15</t>
+  </si>
+  <si>
+    <t>username can not be blank</t>
+  </si>
+  <si>
+    <t>password can not be blank</t>
   </si>
 </sst>
 </file>
@@ -336,49 +342,7 @@
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <fill>
         <patternFill>
@@ -741,8 +705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9E7729A-1ECD-4D18-AD79-215030F792F8}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:C8"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -877,11 +841,23 @@
       <c r="A12" t="s">
         <v>20</v>
       </c>
+      <c r="B12" t="s">
+        <v>87</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
+      <c r="B13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -906,13 +882,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="17" priority="1" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="2" operator="containsText" text="WARNING">
+    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="WARNING">
       <formula>NOT(ISERROR(SEARCH("WARNING",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="3" operator="containsText" text="ERROR">
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="ERROR">
       <formula>NOT(ISERROR(SEARCH("ERROR",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1040,26 +1016,15 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="C1:C2 C4:C1048576">
-    <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="OK">
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="5" operator="containsText" text="WARNING">
+    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="WARNING">
       <formula>NOT(ISERROR(SEARCH("WARNING",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="ERROR">
+    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="ERROR">
       <formula>NOT(ISERROR(SEARCH("ERROR",C1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C3">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="OK">
-      <formula>NOT(ISERROR(SEARCH("OK",C3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="WARNING">
-      <formula>NOT(ISERROR(SEARCH("WARNING",C3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="ERROR">
-      <formula>NOT(ISERROR(SEARCH("ERROR",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1181,13 +1146,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="14" priority="1" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="2" operator="containsText" text="WARNING">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="WARNING">
       <formula>NOT(ISERROR(SEARCH("WARNING",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="3" operator="containsText" text="ERROR">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="ERROR">
       <formula>NOT(ISERROR(SEARCH("ERROR",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1199,7 +1164,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7718E203-9D51-4778-8682-1A55B2CB558B}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B3" sqref="B3:C3"/>
     </sheetView>
   </sheetViews>
@@ -1315,26 +1280,15 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="C1:C2 C4:C1048576">
-    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="OK">
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="WARNING">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="WARNING">
       <formula>NOT(ISERROR(SEARCH("WARNING",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="ERROR">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="ERROR">
       <formula>NOT(ISERROR(SEARCH("ERROR",C1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C3">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="OK">
-      <formula>NOT(ISERROR(SEARCH("OK",C3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="WARNING">
-      <formula>NOT(ISERROR(SEARCH("WARNING",C3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="ERROR">
-      <formula>NOT(ISERROR(SEARCH("ERROR",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adds client-side validation during registration
Implements validation logic to check for empty username, password, confirm password, and code fields during registration.
Provides error messages to the client if any of these fields are missing or passwords do not match.
</commit_message>
<xml_diff>
--- a/ErrorCodes.xlsx
+++ b/ErrorCodes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CtrlPay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{283E9023-256D-44BF-BFCD-43F5BD86C280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48024778-4B72-49A2-9183-DBB4F959E539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="2970" windowWidth="29040" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="3930" windowWidth="28800" windowHeight="14985" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Auth" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="94">
   <si>
     <t>user with the same username already exists</t>
   </si>
@@ -295,6 +295,21 @@
   </si>
   <si>
     <t>password can not be blank</t>
+  </si>
+  <si>
+    <t>username can not be empty</t>
+  </si>
+  <si>
+    <t>password can not be empty</t>
+  </si>
+  <si>
+    <t>confirm password can not be empty</t>
+  </si>
+  <si>
+    <t>passwords do not match</t>
+  </si>
+  <si>
+    <t>code can not be empty</t>
   </si>
 </sst>
 </file>
@@ -705,8 +720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9E7729A-1ECD-4D18-AD79-215030F792F8}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1035,8 +1050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49F1D35A-F5B1-4F7C-BEBF-5839D23DDC9A}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B7" sqref="A1:C17"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1072,25 +1087,55 @@
       <c r="A3" t="s">
         <v>34</v>
       </c>
+      <c r="B3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>35</v>
       </c>
+      <c r="B4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
+      <c r="B5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>37</v>
       </c>
+      <c r="B6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>38</v>
+      </c>
+      <c r="B7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Refactors HTTP request handling
Renames HttpGetter to HttpWorker for clarity and adds a basic HttpPost method.

Adds new error codes to ReturnModel for better error handling.

The renaming reflects a broader role for the class, which is now intended to handle various HTTP operations.
</commit_message>
<xml_diff>
--- a/ErrorCodes.xlsx
+++ b/ErrorCodes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CtrlPay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48024778-4B72-49A2-9183-DBB4F959E539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{261ED89E-B74D-4DA8-9A70-5B8B66B06858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="3930" windowWidth="28800" windowHeight="14985" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="3930" windowWidth="28800" windowHeight="14985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Auth" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="96">
   <si>
     <t>user with the same username already exists</t>
   </si>
@@ -310,6 +310,12 @@
   </si>
   <si>
     <t>code can not be empty</t>
+  </si>
+  <si>
+    <t>http return is null</t>
+  </si>
+  <si>
+    <t>failed to parse http response</t>
   </si>
 </sst>
 </file>
@@ -720,8 +726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9E7729A-1ECD-4D18-AD79-215030F792F8}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,10 +884,22 @@
       <c r="A14" t="s">
         <v>22</v>
       </c>
+      <c r="B14" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1050,7 +1068,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49F1D35A-F5B1-4F7C-BEBF-5839D23DDC9A}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Adds payment processing background service
Adds a background service to automatically pair one-time payments with confirmed transactions.

Implements "Pay from Credit" functionality, allowing users to pay for debts using their available credit. This includes API endpoint, core logic, and frontend integration.

Renames `TransactionHandler` to `PaymentProcessing` to better reflect its purpose.
</commit_message>
<xml_diff>
--- a/ErrorCodes.xlsx
+++ b/ErrorCodes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CtrlPay\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zamos\Documents\GitHub\CtrlPay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{261ED89E-B74D-4DA8-9A70-5B8B66B06858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956343AB-4C47-4631-B005-882B5DBE5739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="3930" windowWidth="28800" windowHeight="14985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="5310" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Auth" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="100">
   <si>
     <t>user with the same username already exists</t>
   </si>
@@ -316,6 +316,18 @@
   </si>
   <si>
     <t>failed to parse http response</t>
+  </si>
+  <si>
+    <t>payment does not exist</t>
+  </si>
+  <si>
+    <t>user does not have permission to pay payment</t>
+  </si>
+  <si>
+    <t>payment is already paid</t>
+  </si>
+  <si>
+    <t>WARNING</t>
   </si>
 </sst>
 </file>
@@ -726,7 +738,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9E7729A-1ECD-4D18-AD79-215030F792F8}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -934,7 +946,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -981,15 +993,33 @@
       <c r="A4" t="s">
         <v>73</v>
       </c>
+      <c r="B4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>74</v>
       </c>
+      <c r="B5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>75</v>
+      </c>
+      <c r="B6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1227,7 +1257,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7718E203-9D51-4778-8682-1A55B2CB558B}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B3" sqref="B3:C3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Adds customer management API
Implements the customer management API endpoints for creating, retrieving, editing, and deleting customer records.

Introduces CustomerApiDTO for data transfer.

Adds role-based authorization checks to ensure only Accountants and Admins can access the customer management features.

Configures JWT authentication settings in appsettings.json.

Changes Role to enum.
</commit_message>
<xml_diff>
--- a/ErrorCodes.xlsx
+++ b/ErrorCodes.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zamos\Documents\GitHub\CtrlPay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956343AB-4C47-4631-B005-882B5DBE5739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B94ED7C-9E62-4EDF-9025-2A7459C45EF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5310" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Auth" sheetId="2" r:id="rId1"/>
-    <sheet name="Payments" sheetId="6" r:id="rId2"/>
-    <sheet name="Register" sheetId="3" r:id="rId3"/>
-    <sheet name="Transactions" sheetId="7" r:id="rId4"/>
+    <sheet name="Customer" sheetId="8" r:id="rId2"/>
+    <sheet name="Payments" sheetId="6" r:id="rId3"/>
+    <sheet name="Register" sheetId="3" r:id="rId4"/>
+    <sheet name="Transactions" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="110">
   <si>
     <t>user with the same username already exists</t>
   </si>
@@ -328,6 +329,36 @@
   </si>
   <si>
     <t>WARNING</t>
+  </si>
+  <si>
+    <t>Customer Error Codes</t>
+  </si>
+  <si>
+    <t>Z#</t>
+  </si>
+  <si>
+    <t>Z0</t>
+  </si>
+  <si>
+    <t>Z1</t>
+  </si>
+  <si>
+    <t>Z2</t>
+  </si>
+  <si>
+    <t>Z3</t>
+  </si>
+  <si>
+    <t>Z4</t>
+  </si>
+  <si>
+    <t>Z5</t>
+  </si>
+  <si>
+    <t>Z6</t>
+  </si>
+  <si>
+    <t>Z7</t>
   </si>
 </sst>
 </file>
@@ -375,7 +406,49 @@
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="18">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -739,7 +812,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -927,13 +1000,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="17" priority="1" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="WARNING">
+    <cfRule type="containsText" dxfId="16" priority="2" operator="containsText" text="WARNING">
       <formula>NOT(ISERROR(SEARCH("WARNING",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="ERROR">
+    <cfRule type="containsText" dxfId="15" priority="3" operator="containsText" text="ERROR">
       <formula>NOT(ISERROR(SEARCH("ERROR",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -942,11 +1015,111 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6640EA26-FE1B-40CD-A6DF-4C2C090AC62C}">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="C1 C3:C1048576">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="OK">
+      <formula>NOT(ISERROR(SEARCH("OK",C1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="WARNING">
+      <formula>NOT(ISERROR(SEARCH("WARNING",C1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="ERROR">
+      <formula>NOT(ISERROR(SEARCH("ERROR",C1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="OK">
+      <formula>NOT(ISERROR(SEARCH("OK",C2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="WARNING">
+      <formula>NOT(ISERROR(SEARCH("WARNING",C2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="ERROR">
+      <formula>NOT(ISERROR(SEARCH("ERROR",C2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB5244BA-F464-4FCB-913B-51EE1447A6F5}">
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1080,13 +1253,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="14" priority="1" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="WARNING">
+    <cfRule type="containsText" dxfId="13" priority="2" operator="containsText" text="WARNING">
       <formula>NOT(ISERROR(SEARCH("WARNING",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="ERROR">
+    <cfRule type="containsText" dxfId="12" priority="3" operator="containsText" text="ERROR">
       <formula>NOT(ISERROR(SEARCH("ERROR",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1094,7 +1267,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49F1D35A-F5B1-4F7C-BEBF-5839D23DDC9A}">
   <dimension ref="A1:C17"/>
   <sheetViews>
@@ -1239,13 +1412,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="WARNING">
+    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="WARNING">
       <formula>NOT(ISERROR(SEARCH("WARNING",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="ERROR">
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="ERROR">
       <formula>NOT(ISERROR(SEARCH("ERROR",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1253,11 +1426,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7718E203-9D51-4778-8682-1A55B2CB558B}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B3" sqref="B3:C3"/>
     </sheetView>
   </sheetViews>
@@ -1374,13 +1547,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="WARNING">
+    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="WARNING">
       <formula>NOT(ISERROR(SEARCH("WARNING",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="ERROR">
+    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="ERROR">
       <formula>NOT(ISERROR(SEARCH("ERROR",C1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updates error code definitions
Refreshes the error code spreadsheet to reflect changes and additions in customer management functionalities.
</commit_message>
<xml_diff>
--- a/ErrorCodes.xlsx
+++ b/ErrorCodes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zamos\Documents\GitHub\CtrlPay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B94ED7C-9E62-4EDF-9025-2A7459C45EF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9EF7215-C2E9-4604-990F-60ACE2FC435E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="111">
   <si>
     <t>user with the same username already exists</t>
   </si>
@@ -359,6 +359,9 @@
   </si>
   <si>
     <t>Z7</t>
+  </si>
+  <si>
+    <t>customer not found</t>
   </si>
 </sst>
 </file>
@@ -1019,7 +1022,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1054,6 +1057,12 @@
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>103</v>
+      </c>
+      <c r="B3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Removes error codes spreadsheet.
Removes the spreadsheet containing error codes.
This file is no longer needed.
</commit_message>
<xml_diff>
--- a/ErrorCodes.xlsx
+++ b/ErrorCodes.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zamos\Documents\GitHub\CtrlPay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9EF7215-C2E9-4604-990F-60ACE2FC435E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956343AB-4C47-4631-B005-882B5DBE5739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="5310" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Auth" sheetId="2" r:id="rId1"/>
-    <sheet name="Customer" sheetId="8" r:id="rId2"/>
-    <sheet name="Payments" sheetId="6" r:id="rId3"/>
-    <sheet name="Register" sheetId="3" r:id="rId4"/>
-    <sheet name="Transactions" sheetId="7" r:id="rId5"/>
+    <sheet name="Payments" sheetId="6" r:id="rId2"/>
+    <sheet name="Register" sheetId="3" r:id="rId3"/>
+    <sheet name="Transactions" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="100">
   <si>
     <t>user with the same username already exists</t>
   </si>
@@ -329,39 +328,6 @@
   </si>
   <si>
     <t>WARNING</t>
-  </si>
-  <si>
-    <t>Customer Error Codes</t>
-  </si>
-  <si>
-    <t>Z#</t>
-  </si>
-  <si>
-    <t>Z0</t>
-  </si>
-  <si>
-    <t>Z1</t>
-  </si>
-  <si>
-    <t>Z2</t>
-  </si>
-  <si>
-    <t>Z3</t>
-  </si>
-  <si>
-    <t>Z4</t>
-  </si>
-  <si>
-    <t>Z5</t>
-  </si>
-  <si>
-    <t>Z6</t>
-  </si>
-  <si>
-    <t>Z7</t>
-  </si>
-  <si>
-    <t>customer not found</t>
   </si>
 </sst>
 </file>
@@ -409,49 +375,7 @@
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <fill>
         <patternFill>
@@ -815,7 +739,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1003,13 +927,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="17" priority="1" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="2" operator="containsText" text="WARNING">
+    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="WARNING">
       <formula>NOT(ISERROR(SEARCH("WARNING",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="3" operator="containsText" text="ERROR">
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="ERROR">
       <formula>NOT(ISERROR(SEARCH("ERROR",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1018,117 +942,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6640EA26-FE1B-40CD-A6DF-4C2C090AC62C}">
-  <dimension ref="A1:C9"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>109</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="C1 C3:C1048576">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="OK">
-      <formula>NOT(ISERROR(SEARCH("OK",C1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="WARNING">
-      <formula>NOT(ISERROR(SEARCH("WARNING",C1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="ERROR">
-      <formula>NOT(ISERROR(SEARCH("ERROR",C1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="OK">
-      <formula>NOT(ISERROR(SEARCH("OK",C2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="WARNING">
-      <formula>NOT(ISERROR(SEARCH("WARNING",C2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="ERROR">
-      <formula>NOT(ISERROR(SEARCH("ERROR",C2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB5244BA-F464-4FCB-913B-51EE1447A6F5}">
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1262,13 +1080,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="14" priority="1" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="2" operator="containsText" text="WARNING">
+    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="WARNING">
       <formula>NOT(ISERROR(SEARCH("WARNING",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="3" operator="containsText" text="ERROR">
+    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="ERROR">
       <formula>NOT(ISERROR(SEARCH("ERROR",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1276,7 +1094,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49F1D35A-F5B1-4F7C-BEBF-5839D23DDC9A}">
   <dimension ref="A1:C17"/>
   <sheetViews>
@@ -1421,13 +1239,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="WARNING">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="WARNING">
       <formula>NOT(ISERROR(SEARCH("WARNING",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="ERROR">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="ERROR">
       <formula>NOT(ISERROR(SEARCH("ERROR",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1435,11 +1253,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7718E203-9D51-4778-8682-1A55B2CB558B}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B3" sqref="B3:C3"/>
     </sheetView>
   </sheetViews>
@@ -1556,13 +1374,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="WARNING">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="WARNING">
       <formula>NOT(ISERROR(SEARCH("WARNING",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="ERROR">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="ERROR">
       <formula>NOT(ISERROR(SEARCH("ERROR",C1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>